<commit_message>
demeaned rs scores (binning)
</commit_message>
<xml_diff>
--- a/Shared_Reward/covariates/Composite_Reward.xlsx
+++ b/Shared_Reward/covariates/Composite_Reward.xlsx
@@ -13,7 +13,16 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Composite_Reward</t>
+  </si>
+  <si>
+    <t>Composite_Reward_Squared</t>
+  </si>
   <si>
     <t>Subject</t>
   </si>
@@ -60,7 +69,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -71,15 +80,17 @@
     <border/>
     <border/>
     <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -99,13 +110,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2">
@@ -113,10 +124,10 @@
         <v>1003</v>
       </c>
       <c r="B2" s="0">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C2" s="0">
-        <v>25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -124,10 +135,10 @@
         <v>1006</v>
       </c>
       <c r="B3" s="0">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C3" s="0">
-        <v>25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -135,10 +146,10 @@
         <v>1009</v>
       </c>
       <c r="B4" s="0">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C4" s="0">
-        <v>36</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -146,10 +157,10 @@
         <v>1010</v>
       </c>
       <c r="B5" s="0">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C5" s="0">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -157,10 +168,10 @@
         <v>1011</v>
       </c>
       <c r="B6" s="0">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C6" s="0">
-        <v>49</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -168,10 +179,10 @@
         <v>1012</v>
       </c>
       <c r="B7" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -179,10 +190,10 @@
         <v>1013</v>
       </c>
       <c r="B8" s="0">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="C8" s="0">
-        <v>81</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -190,10 +201,10 @@
         <v>1015</v>
       </c>
       <c r="B9" s="0">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C9" s="0">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -201,10 +212,10 @@
         <v>1016</v>
       </c>
       <c r="B10" s="0">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C10" s="0">
-        <v>64</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -212,10 +223,10 @@
         <v>1019</v>
       </c>
       <c r="B11" s="0">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C11" s="0">
-        <v>64</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -223,10 +234,10 @@
         <v>1021</v>
       </c>
       <c r="B12" s="0">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C12" s="0">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -234,10 +245,10 @@
         <v>1242</v>
       </c>
       <c r="B13" s="0">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C13" s="0">
-        <v>49</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -245,10 +256,10 @@
         <v>1244</v>
       </c>
       <c r="B14" s="0">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C14" s="0">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -256,10 +267,10 @@
         <v>1245</v>
       </c>
       <c r="B15" s="0">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C15" s="0">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
@@ -267,10 +278,10 @@
         <v>1247</v>
       </c>
       <c r="B16" s="0">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C16" s="0">
-        <v>64</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -278,10 +289,10 @@
         <v>1248</v>
       </c>
       <c r="B17" s="0">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C17" s="0">
-        <v>49</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -289,10 +300,10 @@
         <v>1249</v>
       </c>
       <c r="B18" s="0">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C18" s="0">
-        <v>49</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
@@ -300,10 +311,10 @@
         <v>1251</v>
       </c>
       <c r="B19" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C19" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
@@ -311,10 +322,10 @@
         <v>1253</v>
       </c>
       <c r="B20" s="0">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="C20" s="0">
-        <v>81</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
@@ -322,10 +333,10 @@
         <v>1255</v>
       </c>
       <c r="B21" s="0">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C21" s="0">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22">
@@ -333,10 +344,10 @@
         <v>1276</v>
       </c>
       <c r="B22" s="0">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C22" s="0">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23">
@@ -344,10 +355,10 @@
         <v>1282</v>
       </c>
       <c r="B23" s="0">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="C23" s="0">
-        <v>81</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24">
@@ -355,10 +366,10 @@
         <v>1286</v>
       </c>
       <c r="B24" s="0">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C24" s="0">
-        <v>25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
@@ -366,10 +377,10 @@
         <v>1294</v>
       </c>
       <c r="B25" s="0">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C25" s="0">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26">
@@ -377,10 +388,10 @@
         <v>1300</v>
       </c>
       <c r="B26" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C26" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27">
@@ -388,10 +399,10 @@
         <v>1301</v>
       </c>
       <c r="B27" s="0">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C27" s="0">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28">
@@ -399,10 +410,10 @@
         <v>1302</v>
       </c>
       <c r="B28" s="0">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C28" s="0">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29">
@@ -410,10 +421,10 @@
         <v>1303</v>
       </c>
       <c r="B29" s="0">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C29" s="0">
-        <v>36</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30">
@@ -421,10 +432,10 @@
         <v>3101</v>
       </c>
       <c r="B30" s="0">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C30" s="0">
-        <v>25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31">
@@ -432,10 +443,10 @@
         <v>3116</v>
       </c>
       <c r="B31" s="0">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C31" s="0">
-        <v>49</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32">
@@ -443,10 +454,10 @@
         <v>3122</v>
       </c>
       <c r="B32" s="0">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="C32" s="0">
-        <v>81</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33">
@@ -454,10 +465,10 @@
         <v>3125</v>
       </c>
       <c r="B33" s="0">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C33" s="0">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34">
@@ -465,10 +476,10 @@
         <v>3140</v>
       </c>
       <c r="B34" s="0">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C34" s="0">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35">
@@ -476,10 +487,10 @@
         <v>3143</v>
       </c>
       <c r="B35" s="0">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C35" s="0">
-        <v>36</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36">
@@ -487,10 +498,10 @@
         <v>3152</v>
       </c>
       <c r="B36" s="0">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C36" s="0">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37">
@@ -498,10 +509,10 @@
         <v>3164</v>
       </c>
       <c r="B37" s="0">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C37" s="0">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38">
@@ -509,10 +520,10 @@
         <v>3166</v>
       </c>
       <c r="B38" s="0">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C38" s="0">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39">
@@ -520,10 +531,10 @@
         <v>3167</v>
       </c>
       <c r="B39" s="0">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C39" s="0">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40">
@@ -531,10 +542,10 @@
         <v>3170</v>
       </c>
       <c r="B40" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C40" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41">
@@ -542,10 +553,10 @@
         <v>3173</v>
       </c>
       <c r="B41" s="0">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="C41" s="0">
-        <v>81</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42">
@@ -553,10 +564,10 @@
         <v>3175</v>
       </c>
       <c r="B42" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C42" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43">
@@ -564,10 +575,10 @@
         <v>3176</v>
       </c>
       <c r="B43" s="0">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C43" s="0">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44">
@@ -575,10 +586,10 @@
         <v>3189</v>
       </c>
       <c r="B44" s="0">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C44" s="0">
-        <v>25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45">
@@ -586,10 +597,10 @@
         <v>3190</v>
       </c>
       <c r="B45" s="0">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="C45" s="0">
-        <v>81</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46">
@@ -597,10 +608,10 @@
         <v>3199</v>
       </c>
       <c r="B46" s="0">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C46" s="0">
-        <v>36</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47">
@@ -608,10 +619,10 @@
         <v>3200</v>
       </c>
       <c r="B47" s="0">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C47" s="0">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48">
@@ -619,10 +630,10 @@
         <v>3206</v>
       </c>
       <c r="B48" s="0">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C48" s="0">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49">
@@ -630,10 +641,10 @@
         <v>3210</v>
       </c>
       <c r="B49" s="0">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C49" s="0">
-        <v>64</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50">
@@ -641,10 +652,10 @@
         <v>3212</v>
       </c>
       <c r="B50" s="0">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C50" s="0">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51">
@@ -652,10 +663,10 @@
         <v>3220</v>
       </c>
       <c r="B51" s="0">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C51" s="0">
-        <v>36</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>